<commit_message>
This is a running code with 3 functionalities 1. Get Status	2. Issue Book	3. Return Book Should try maps and other features like password check and new user registeration.
</commit_message>
<xml_diff>
--- a/UsersInfo.xlsx
+++ b/UsersInfo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>SerNo</t>
   </si>
@@ -71,12 +71,16 @@
   </si>
   <si>
     <t>khandya</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -420,12 +424,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.21875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.77734375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.21875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -465,20 +469,18 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
         <v>14</v>
       </c>
+      <c r="H2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -508,11 +510,15 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
20Nov2015 Working code with sqlite database
</commit_message>
<xml_diff>
--- a/UsersInfo.xlsx
+++ b/UsersInfo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>SerNo</t>
   </si>
@@ -480,7 +480,9 @@
       <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="H2"/>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -493,11 +495,12 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">

</xml_diff>